<commit_message>
80% through making a SimpleCow
</commit_message>
<xml_diff>
--- a/Tests/Simulation/SoilNitrogenPatch/SimpleCowParameters.xlsx
+++ b/Tests/Simulation/SoilNitrogenPatch/SimpleCowParameters.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aaUnderVC\ApsimX\Tests\Simulation\SoilNitrogenPatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66829199-6CAB-4C6A-AA63-56BB0E5817D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77007BF5-1EF6-43EE-A59A-02C803C777ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="0" windowWidth="38040" windowHeight="21000" activeTab="1" xr2:uid="{4D7A34B9-F399-49ED-8EFB-93F74E449795}"/>
+    <workbookView xWindow="2400" yWindow="3255" windowWidth="18945" windowHeight="16860" activeTab="3" xr2:uid="{4D7A34B9-F399-49ED-8EFB-93F74E449795}"/>
   </bookViews>
   <sheets>
     <sheet name="Woods Parameter" sheetId="1" r:id="rId1"/>
     <sheet name="Prgnancy parameter" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Prgnancy parameter'!$T$2:$U$2,'Prgnancy parameter'!$N$4</definedName>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>P0</t>
   </si>
@@ -109,6 +110,30 @@
   </si>
   <si>
     <t>C2</t>
+  </si>
+  <si>
+    <t>exported</t>
+  </si>
+  <si>
+    <t>urine</t>
+  </si>
+  <si>
+    <t>dung</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>DryStock</t>
+  </si>
+  <si>
+    <t>Fraction of defoliated biomass …</t>
+  </si>
+  <si>
+    <t>Fraction of defoliated N ,,,</t>
+  </si>
+  <si>
+    <t>Proportion of excreted N going to dung</t>
   </si>
 </sst>
 </file>
@@ -1967,553 +1992,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Prgnancy parameter'!$N$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Epreg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Prgnancy parameter'!$M$9:$M$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Prgnancy parameter'!$N$9:$N$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B43F-4596-AC82-DF0F3AEEF2CF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Prgnancy parameter'!$O$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Epreg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Prgnancy parameter'!$M$9:$M$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Prgnancy parameter'!$O$9:$O$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>48</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B43F-4596-AC82-DF0F3AEEF2CF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Prgnancy parameter'!$P$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Epreg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Prgnancy parameter'!$M$9:$M$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Prgnancy parameter'!$P$9:$P$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B43F-4596-AC82-DF0F3AEEF2CF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Prgnancy parameter'!$Q$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Epreg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Prgnancy parameter'!$M$9:$M$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Prgnancy parameter'!$Q$9:$Q$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>57</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B43F-4596-AC82-DF0F3AEEF2CF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="446660320"/>
-        <c:axId val="446658160"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="446660320"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="446658160"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="446658160"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="446660320"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
     <c:title>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2857,7 +2335,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3035,6 +2513,382 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>42.44481492015354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C969-4ACA-9210-C66D74065316}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="446660320"/>
+        <c:axId val="446658160"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="446660320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446658160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="446658160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446660320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prgnancy parameter'!$N$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Epreg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Prgnancy parameter'!$M$9:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Prgnancy parameter'!$Q$9:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B43F-4596-AC82-DF0F3AEEF2CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prgnancy parameter'!$N$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Prgnancy parameter'!$M$9:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Prgnancy parameter'!$Q$16:$Q$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14.240835509171314</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.931039107146443</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.64608456868794</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.749435684631983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3312,21 +3166,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Prgnancy parameter'!$Q$9:$Q$12</c:f>
+              <c:f>'Prgnancy parameter'!$P$9:$P$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3396,21 +3250,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Prgnancy parameter'!$Q$16:$Q$19</c:f>
+              <c:f>'Prgnancy parameter'!$P$16:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14.240835509171314</c:v>
+                  <c:v>12.982811170905297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.931039107146443</c:v>
+                  <c:v>22.728650493440927</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.64608456868794</c:v>
+                  <c:v>39.790423387708444</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57.749435684631983</c:v>
+                  <c:v>52.647895429805835</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3627,90 +3481,302 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Prgnancy parameter'!$N$8</c:f>
+              <c:f>'Prgnancy parameter'!$N$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Epreg</c:v>
+                  <c:v>Wt25</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Prgnancy parameter'!$M$9:$M$12</c:f>
+              <c:f>'Prgnancy parameter'!$M$29:$M$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="29">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="33">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="37">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Prgnancy parameter'!$P$9:$P$12</c:f>
+              <c:f>'Prgnancy parameter'!$N$29:$N$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>0.20767202631768128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>0.23887969062881723</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>0.27477704920944895</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>0.31606884023293202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.36356570555513262</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4182001052631108</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.48104462376349066</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55333302679627627</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.63648448276612046</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.73213142390506247</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.84215159423802777</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.96870491351784616</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1142758808438349</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2817223504332211</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4743316371130351</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6958850529974061</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.9507321423365167</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.2438760719183226</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5810718534103225</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.968939325945755</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.4150931170322401</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.9282921331798444</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.5186115150537391</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.1976404329808767</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.9787096059388372</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.8771530106874632</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.9106089189258855</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.0993661724467412</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.466762494373262</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12.039642656139081</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>13.848885494960616</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.930010128227098</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>18.323873266029896</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>21.077471311494595</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>24.244862995777112</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>27.888230660925554</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>32.079101025749438</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>36.899749400813583</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42.44481492015354</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>48.823158499996936</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>56.16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B43F-4596-AC82-DF0F3AEEF2CF}"/>
+              <c16:uniqueId val="{00000000-F334-420B-BADF-BA52318A73B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3719,14 +3785,17 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Prgnancy parameter'!$N$15</c:f>
+              <c:f>'Prgnancy parameter'!$O$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wt30</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -3735,66 +3804,870 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Prgnancy parameter'!$M$9:$M$12</c:f>
+              <c:f>'Prgnancy parameter'!$M$29:$M$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="29">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="33">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="37">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Prgnancy parameter'!$P$16:$P$19</c:f>
+              <c:f>'Prgnancy parameter'!$O$29:$O$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>12.982811170905297</c:v>
+                  <c:v>0.23263260640394104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.728650493440927</c:v>
+                  <c:v>0.2675911919063193</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.790423387708444</c:v>
+                  <c:v>0.30780313685481542</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52.647895429805835</c:v>
+                  <c:v>0.35405788353015943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40726350670358608</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46846454099185009</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53886248719660257</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.61983940020929029</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.71298502156012533</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82012798927826713</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.94337173777625227</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0851357925464336</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2482032703683343</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4357755175525986</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6515349588814288</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8997173910980558</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1851951402135019</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5135727151777365</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.8912968357913709</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.3257829949296198</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.8255610397524613</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.4004426299562684</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.0617138606130831</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.8223568311756937</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.6973045104987934</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.7037339013950916</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.8614032601429393</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.193039991250435</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>11.724786832639278</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>13.486715090771181</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15.513415001566459</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>17.844674807100546</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20.526261879735411</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>23.610821228741543</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>27.1589090289234</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>31.240181461517569</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>35.934762206728941</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41.334815434565215</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>47.546355174979688</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>54.691326588938871</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>62.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C969-4ACA-9210-C66D74065316}"/>
+              <c16:uniqueId val="{00000001-F334-420B-BADF-BA52318A73B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prgnancy parameter'!$P$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wt35</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Prgnancy parameter'!$M$29:$M$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Prgnancy parameter'!$P$29:$P$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0.2575931864902008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29630269318382135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.34082922450018188</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39204692682738679</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45096130785203953</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.51872897672058937</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.59668035062971436</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68634577362230431</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78948556035413009</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90812455465147179</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0445918813144768</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2015666715750208</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3821306598928338</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.5898286846719762</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8287382806498222</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.1035497291987055</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.4196581380904871</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.7832693584371504</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.2015218181724192</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6826266639134846</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.2360289624726821</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.8725931267326921</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.6048162061724263</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.4470732293705106</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.4158994150587496</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.5303147921027183</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.8121976013599923</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>11.286713810054131</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12.982811170905297</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.933787525403282</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17.177944508172303</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.759339485973996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>22.728650493440927</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>26.144171145988491</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30.072955062069688</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>34.59213226210958</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>39.790423387708444</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>45.769881468316854</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>52.647895429805835</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>60.559494677880814</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>69.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F334-420B-BADF-BA52318A73B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Prgnancy parameter'!$Q$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wt40</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Prgnancy parameter'!$M$29:$M$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Prgnancy parameter'!$Q$29:$Q$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0.28255376657646059</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32501419446132346</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.37385531214554835</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4300359701246142</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.49465910900049292</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56899341244932866</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65449821406282627</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.75285214703531833</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.86598609914813496</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99612112002467645</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1458120248527013</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3179975506036081</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.516058049417333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7438818517913537</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0059416024182162</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.3073820672993555</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6541211359674723</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.0529660016965638</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5117468005534676</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.0394703328973494</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.6464968851929038</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.3447436235091157</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.1479185517317703</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.0717896275653276</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.1344943196187067</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.3568956828103467</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.762991942577045</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12.380387628857825</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14.240835509171314</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16.380859960035384</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18.842474014778148</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>21.674004164847446</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>24.931039107146443</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>28.677521063235435</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>32.987001095215973</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37.944083062701594</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>43.64608456868794</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>50.204947502068485</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>57.749435684631983</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>66.427662766822749</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>76.41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F334-420B-BADF-BA52318A73B9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3806,11 +4679,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="446660320"/>
-        <c:axId val="446658160"/>
+        <c:axId val="1039118840"/>
+        <c:axId val="1039121720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="446660320"/>
+        <c:axId val="1039118840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3867,12 +4740,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="446658160"/>
+        <c:crossAx val="1039121720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="446658160"/>
+        <c:axId val="1039121720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3929,7 +4802,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="446660320"/>
+        <c:crossAx val="1039118840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7958,16 +8831,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>304004</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>47267</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>580229</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>142517</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7990,7 +8863,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15687675" y="1752600"/>
+          <a:off x="17373600" y="6991350"/>
           <a:ext cx="6371429" cy="2866667"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8002,52 +8875,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25854971-D76B-C536-A8EE-DCCD9A0571BA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8066,7 +8903,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8102,7 +8939,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8138,7 +8975,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8163,6 +9000,42 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D427CE23-CF73-2D2D-B90D-F963E201D491}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8863E144-9D6D-47AA-0F37-593686434ADA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8701,7 +9574,7 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:I75" si="2">$B$1*$D12^$B$2*EXP(-1*$B$3*$D12)*E$2</f>
+        <f t="shared" ref="E12:I49" si="2">$B$1*$D12^$B$2*EXP(-1*$B$3*$D12)*E$2</f>
         <v>1.7678525680402746</v>
       </c>
       <c r="F12">
@@ -8752,7 +9625,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
-        <f t="shared" ref="C14:C55" si="3">C13+7</f>
+        <f t="shared" ref="C14:C49" si="3">C13+7</f>
         <v>45519</v>
       </c>
       <c r="D14">
@@ -9828,10 +10701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9FBD8C-36ED-4BEA-951C-3E3AC98BA8A4}">
-  <dimension ref="D1:U52"/>
+  <dimension ref="D1:U69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10054,7 +10927,7 @@
         <v>39</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:H49" si="4">E$3*EXP(E$4*$D10)</f>
+        <f t="shared" ref="E10:H48" si="4">E$3*EXP(E$4*$D10)</f>
         <v>0.28219716541600681</v>
       </c>
       <c r="F10">
@@ -10251,7 +11124,7 @@
         <v>10.466762494373262</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16:Q20" si="5">O$3*EXP(O$4*$M16)</f>
+        <f t="shared" ref="O16:Q19" si="5">O$3*EXP(O$4*$M16)</f>
         <v>11.724786832639278</v>
       </c>
       <c r="P16">
@@ -10287,7 +11160,7 @@
         <v>8</v>
       </c>
       <c r="N17">
-        <f t="shared" ref="N17:Q20" si="6">N$3*EXP(N$4*$M17)</f>
+        <f t="shared" ref="N17:N19" si="6">N$3*EXP(N$4*$M17)</f>
         <v>18.323873266029896</v>
       </c>
       <c r="O17">
@@ -10651,6 +11524,25 @@
         <f t="shared" si="4"/>
         <v>3.8630863790918855</v>
       </c>
+      <c r="M28" t="s">
+        <v>11</v>
+      </c>
+      <c r="N28" t="str">
+        <f>"Wt"&amp;N1</f>
+        <v>Wt25</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" ref="O28:Q28" si="11">"Wt"&amp;O1</f>
+        <v>Wt30</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="11"/>
+        <v>Wt35</v>
+      </c>
+      <c r="Q28" t="str">
+        <f t="shared" si="11"/>
+        <v>Wt40</v>
+      </c>
     </row>
     <row r="29" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D29">
@@ -10672,6 +11564,25 @@
         <f t="shared" si="4"/>
         <v>4.452503151822679</v>
       </c>
+      <c r="M29">
+        <v>40</v>
+      </c>
+      <c r="N29">
+        <f>N$3*EXP(N$4*$M29)</f>
+        <v>0.20767202631768128</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:Q44" si="12">O$3*EXP(O$4*$M29)</f>
+        <v>0.23263260640394104</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="12"/>
+        <v>0.2575931864902008</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="12"/>
+        <v>0.28255376657646059</v>
+      </c>
     </row>
     <row r="30" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D30">
@@ -10693,6 +11604,25 @@
         <f t="shared" si="4"/>
         <v>5.1318511603282344</v>
       </c>
+      <c r="M30">
+        <v>39</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ref="N30:Q69" si="13">N$3*EXP(N$4*$M30)</f>
+        <v>0.23887969062881723</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="12"/>
+        <v>0.2675911919063193</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="12"/>
+        <v>0.29630269318382135</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="12"/>
+        <v>0.32501419446132346</v>
+      </c>
     </row>
     <row r="31" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D31">
@@ -10714,6 +11644,25 @@
         <f t="shared" si="4"/>
         <v>5.9148518111618591</v>
       </c>
+      <c r="M31">
+        <v>38</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="13"/>
+        <v>0.27477704920944895</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="12"/>
+        <v>0.30780313685481542</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="12"/>
+        <v>0.34082922450018188</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="12"/>
+        <v>0.37385531214554835</v>
+      </c>
     </row>
     <row r="32" spans="4:19" x14ac:dyDescent="0.25">
       <c r="D32">
@@ -10735,8 +11684,27 @@
         <f t="shared" si="4"/>
         <v>6.8173200771019689</v>
       </c>
-    </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>37</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="13"/>
+        <v>0.31606884023293202</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="12"/>
+        <v>0.35405788353015943</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="12"/>
+        <v>0.39204692682738679</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="12"/>
+        <v>0.4300359701246142</v>
+      </c>
+    </row>
+    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>16</v>
       </c>
@@ -10756,8 +11724,27 @@
         <f t="shared" si="4"/>
         <v>7.8574839264702216</v>
       </c>
-    </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>36</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="13"/>
+        <v>0.36356570555513262</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="12"/>
+        <v>0.40726350670358608</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="12"/>
+        <v>0.45096130785203953</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="12"/>
+        <v>0.49465910900049292</v>
+      </c>
+    </row>
+    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>15</v>
       </c>
@@ -10777,8 +11764,27 @@
         <f t="shared" si="4"/>
         <v>9.0563524899044339</v>
       </c>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>35</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="13"/>
+        <v>0.4182001052631108</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="12"/>
+        <v>0.46846454099185009</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="12"/>
+        <v>0.51872897672058937</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="12"/>
+        <v>0.56899341244932866</v>
+      </c>
+    </row>
+    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>14</v>
       </c>
@@ -10798,8 +11804,27 @@
         <f t="shared" si="4"/>
         <v>10.438140400783816</v>
       </c>
-    </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>34</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="13"/>
+        <v>0.48104462376349066</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="12"/>
+        <v>0.53886248719660257</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="12"/>
+        <v>0.59668035062971436</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="12"/>
+        <v>0.65449821406282627</v>
+      </c>
+    </row>
+    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>13</v>
       </c>
@@ -10819,8 +11844,27 @@
         <f t="shared" si="4"/>
         <v>12.030756880094119</v>
       </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>33</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="13"/>
+        <v>0.55333302679627627</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="12"/>
+        <v>0.61983940020929029</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="12"/>
+        <v>0.68634577362230431</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="12"/>
+        <v>0.75285214703531833</v>
+      </c>
+    </row>
+    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>12</v>
       </c>
@@ -10840,8 +11884,27 @@
         <f t="shared" si="4"/>
         <v>13.866369444222395</v>
       </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>32</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="13"/>
+        <v>0.63648448276612046</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="12"/>
+        <v>0.71298502156012533</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="12"/>
+        <v>0.78948556035413009</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="12"/>
+        <v>0.86598609914813496</v>
+      </c>
+    </row>
+    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>11</v>
       </c>
@@ -10861,8 +11924,27 @@
         <f t="shared" si="4"/>
         <v>15.98205362139778</v>
       </c>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>31</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="13"/>
+        <v>0.73213142390506247</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="12"/>
+        <v>0.82012798927826713</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="12"/>
+        <v>0.90812455465147179</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="12"/>
+        <v>0.99612112002467645</v>
+      </c>
+    </row>
+    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>10</v>
       </c>
@@ -10882,8 +11964,27 @@
         <f t="shared" si="4"/>
         <v>18.420541799689353</v>
       </c>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>30</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="13"/>
+        <v>0.84215159423802777</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="12"/>
+        <v>0.94337173777625227</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="12"/>
+        <v>1.0445918813144768</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="12"/>
+        <v>1.1458120248527013</v>
+      </c>
+    </row>
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>9</v>
       </c>
@@ -10903,8 +12004,27 @@
         <f t="shared" si="4"/>
         <v>21.23108633172177</v>
       </c>
-    </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>29</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="13"/>
+        <v>0.96870491351784616</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="12"/>
+        <v>1.0851357925464336</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="12"/>
+        <v>1.2015666715750208</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="12"/>
+        <v>1.3179975506036081</v>
+      </c>
+    </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>8</v>
       </c>
@@ -10924,8 +12044,27 @@
         <f t="shared" si="4"/>
         <v>24.470454329015688</v>
       </c>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>28</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="13"/>
+        <v>1.1142758808438349</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="12"/>
+        <v>1.2482032703683343</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="12"/>
+        <v>1.3821306598928338</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="12"/>
+        <v>1.516058049417333</v>
+      </c>
+    </row>
+    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>7</v>
       </c>
@@ -10945,8 +12084,27 @@
         <f t="shared" si="4"/>
         <v>28.20407423871475</v>
       </c>
-    </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>27</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="13"/>
+        <v>1.2817223504332211</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="12"/>
+        <v>1.4357755175525986</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="12"/>
+        <v>1.5898286846719762</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="12"/>
+        <v>1.7438818517913537</v>
+      </c>
+    </row>
+    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D43">
         <v>6</v>
       </c>
@@ -10966,8 +12124,27 @@
         <f t="shared" si="4"/>
         <v>32.507357361146731</v>
       </c>
-    </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>26</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="13"/>
+        <v>1.4743316371130351</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="12"/>
+        <v>1.6515349588814288</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="12"/>
+        <v>1.8287382806498222</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="12"/>
+        <v>2.0059416024182162</v>
+      </c>
+    </row>
+    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D44">
         <v>5</v>
       </c>
@@ -10987,8 +12164,27 @@
         <f t="shared" si="4"/>
         <v>37.467221000105226</v>
       </c>
-    </row>
-    <row r="45" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>25</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="13"/>
+        <v>1.6958850529974061</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="12"/>
+        <v>1.8997173910980558</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="12"/>
+        <v>2.1035497291987055</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="12"/>
+        <v>2.3073820672993555</v>
+      </c>
+    </row>
+    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D45">
         <v>4</v>
       </c>
@@ -11008,8 +12204,27 @@
         <f t="shared" si="4"/>
         <v>43.183844010296575</v>
       </c>
-    </row>
-    <row r="46" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>24</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="13"/>
+        <v>1.9507321423365167</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="13"/>
+        <v>2.1851951402135019</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="13"/>
+        <v>2.4196581380904871</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="13"/>
+        <v>2.6541211359674723</v>
+      </c>
+    </row>
+    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D46">
         <v>3</v>
       </c>
@@ -11029,8 +12244,27 @@
         <f t="shared" si="4"/>
         <v>49.772690200332448</v>
       </c>
-    </row>
-    <row r="47" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>23</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="13"/>
+        <v>2.2438760719183226</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="13"/>
+        <v>2.5135727151777365</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="13"/>
+        <v>2.7832693584371504</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="13"/>
+        <v>3.0529660016965638</v>
+      </c>
+    </row>
+    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D47">
         <v>2</v>
       </c>
@@ -11050,8 +12284,27 @@
         <f t="shared" si="4"/>
         <v>57.366840459769804</v>
       </c>
-    </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>22</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="13"/>
+        <v>2.5810718534103225</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="13"/>
+        <v>2.8912968357913709</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="13"/>
+        <v>3.2015218181724192</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="13"/>
+        <v>3.5117468005534676</v>
+      </c>
+    </row>
+    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D48">
         <v>1</v>
       </c>
@@ -11071,11 +12324,535 @@
         <f t="shared" si="4"/>
         <v>66.11968071427853</v>
       </c>
-    </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>21</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="13"/>
+        <v>2.968939325945755</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="13"/>
+        <v>3.3257829949296198</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="13"/>
+        <v>3.6826266639134846</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="13"/>
+        <v>4.0394703328973494</v>
+      </c>
+    </row>
+    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>20</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="13"/>
+        <v>3.4150931170322401</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="13"/>
+        <v>3.8255610397524613</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="13"/>
+        <v>4.2360289624726821</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="13"/>
+        <v>4.6464968851929038</v>
+      </c>
+    </row>
+    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>19</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="13"/>
+        <v>3.9282921331798444</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="13"/>
+        <v>4.4004426299562684</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="13"/>
+        <v>4.8725931267326921</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="13"/>
+        <v>5.3447436235091157</v>
+      </c>
+    </row>
+    <row r="51" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <v>18</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="13"/>
+        <v>4.5186115150537391</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="13"/>
+        <v>5.0617138606130831</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="13"/>
+        <v>5.6048162061724263</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="13"/>
+        <v>6.1479185517317703</v>
+      </c>
+    </row>
+    <row r="52" spans="4:17" x14ac:dyDescent="0.25">
       <c r="M52">
-        <f>9*7</f>
-        <v>63</v>
+        <v>17</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="13"/>
+        <v>5.1976404329808767</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="13"/>
+        <v>5.8223568311756937</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="13"/>
+        <v>6.4470732293705106</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="13"/>
+        <v>7.0717896275653276</v>
+      </c>
+    </row>
+    <row r="53" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="M53">
+        <v>16</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="13"/>
+        <v>5.9787096059388372</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="13"/>
+        <v>6.6973045104987934</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="13"/>
+        <v>7.4158994150587496</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="13"/>
+        <v>8.1344943196187067</v>
+      </c>
+    </row>
+    <row r="54" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="M54">
+        <v>15</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="13"/>
+        <v>6.8771530106874632</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="13"/>
+        <v>7.7037339013950916</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="13"/>
+        <v>8.5303147921027183</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="13"/>
+        <v>9.3568956828103467</v>
+      </c>
+    </row>
+    <row r="55" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>280</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ref="E55" si="14">D55/7</f>
+        <v>40</v>
+      </c>
+      <c r="M55">
+        <v>14</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="13"/>
+        <v>7.9106089189258855</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="13"/>
+        <v>8.8614032601429393</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="13"/>
+        <v>9.8121976013599923</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="13"/>
+        <v>10.762991942577045</v>
+      </c>
+    </row>
+    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>281</v>
+      </c>
+      <c r="E56">
+        <f>D56/7</f>
+        <v>40.142857142857146</v>
+      </c>
+      <c r="M56">
+        <v>13</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="13"/>
+        <v>9.0993661724467412</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="13"/>
+        <v>10.193039991250435</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="13"/>
+        <v>11.286713810054131</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="13"/>
+        <v>12.380387628857825</v>
+      </c>
+    </row>
+    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>282</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ref="E57:E64" si="15">D57/7</f>
+        <v>40.285714285714285</v>
+      </c>
+      <c r="M57">
+        <v>12</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="13"/>
+        <v>10.466762494373262</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="13"/>
+        <v>11.724786832639278</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="13"/>
+        <v>12.982811170905297</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="13"/>
+        <v>14.240835509171314</v>
+      </c>
+    </row>
+    <row r="58" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>283</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="15"/>
+        <v>40.428571428571431</v>
+      </c>
+      <c r="M58">
+        <v>11</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="13"/>
+        <v>12.039642656139081</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="13"/>
+        <v>13.486715090771181</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="13"/>
+        <v>14.933787525403282</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="13"/>
+        <v>16.380859960035384</v>
+      </c>
+    </row>
+    <row r="59" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>284</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="15"/>
+        <v>40.571428571428569</v>
+      </c>
+      <c r="M59">
+        <v>10</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="13"/>
+        <v>13.848885494960616</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="13"/>
+        <v>15.513415001566459</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="13"/>
+        <v>17.177944508172303</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="13"/>
+        <v>18.842474014778148</v>
+      </c>
+    </row>
+    <row r="60" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>285</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="15"/>
+        <v>40.714285714285715</v>
+      </c>
+      <c r="M60">
+        <v>9</v>
+      </c>
+      <c r="N60">
+        <f t="shared" si="13"/>
+        <v>15.930010128227098</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="13"/>
+        <v>17.844674807100546</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="13"/>
+        <v>19.759339485973996</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="13"/>
+        <v>21.674004164847446</v>
+      </c>
+    </row>
+    <row r="61" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>286</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="15"/>
+        <v>40.857142857142854</v>
+      </c>
+      <c r="M61">
+        <v>8</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="13"/>
+        <v>18.323873266029896</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="13"/>
+        <v>20.526261879735411</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="13"/>
+        <v>22.728650493440927</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="13"/>
+        <v>24.931039107146443</v>
+      </c>
+    </row>
+    <row r="62" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>287</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="15"/>
+        <v>41</v>
+      </c>
+      <c r="M62">
+        <v>7</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="13"/>
+        <v>21.077471311494595</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="13"/>
+        <v>23.610821228741543</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="13"/>
+        <v>26.144171145988491</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="13"/>
+        <v>28.677521063235435</v>
+      </c>
+    </row>
+    <row r="63" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>288</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="15"/>
+        <v>41.142857142857146</v>
+      </c>
+      <c r="M63">
+        <v>6</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="13"/>
+        <v>24.244862995777112</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="13"/>
+        <v>27.1589090289234</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="13"/>
+        <v>30.072955062069688</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="13"/>
+        <v>32.987001095215973</v>
+      </c>
+    </row>
+    <row r="64" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>289</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="15"/>
+        <v>41.285714285714285</v>
+      </c>
+      <c r="M64">
+        <v>5</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="13"/>
+        <v>27.888230660925554</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="13"/>
+        <v>31.240181461517569</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="13"/>
+        <v>34.59213226210958</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="13"/>
+        <v>37.944083062701594</v>
+      </c>
+    </row>
+    <row r="65" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M65">
+        <v>4</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="13"/>
+        <v>32.079101025749438</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="13"/>
+        <v>35.934762206728941</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="13"/>
+        <v>39.790423387708444</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="13"/>
+        <v>43.64608456868794</v>
+      </c>
+    </row>
+    <row r="66" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M66">
+        <v>3</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="13"/>
+        <v>36.899749400813583</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="13"/>
+        <v>41.334815434565215</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="13"/>
+        <v>45.769881468316854</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="13"/>
+        <v>50.204947502068485</v>
+      </c>
+    </row>
+    <row r="67" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M67">
+        <v>2</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="13"/>
+        <v>42.44481492015354</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="13"/>
+        <v>47.546355174979688</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="13"/>
+        <v>52.647895429805835</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="13"/>
+        <v>57.749435684631983</v>
+      </c>
+    </row>
+    <row r="68" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <v>1</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="13"/>
+        <v>48.823158499996936</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="13"/>
+        <v>54.691326588938871</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="13"/>
+        <v>60.559494677880814</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="13"/>
+        <v>66.427662766822749</v>
+      </c>
+    </row>
+    <row r="69" spans="13:17" x14ac:dyDescent="0.25">
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="13"/>
+        <v>56.16</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="13"/>
+        <v>62.91</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="13"/>
+        <v>69.66</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="13"/>
+        <v>76.41</v>
       </c>
     </row>
   </sheetData>
@@ -11086,15 +12863,154 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A97C0FC-A5C4-473A-B981-9D6C1FEA780D}">
+  <dimension ref="A16:E45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>0.4*D16</f>
+        <v>6.16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f>D17/D18</f>
+        <v>2.124137931034483</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32">
+        <f>A32/SUM(A31:A32)</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>0.8</v>
+      </c>
+      <c r="C37">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>0.3</v>
+      </c>
+      <c r="C38">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f>C42*C43</f>
+        <v>154000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f>C44/1000</f>
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C11A338-C235-4EB1-9B2D-F22D6696DA63}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>